<commit_message>
✅ Veri Güncellendi: Istanbul
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -521,19 +521,19 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Eczane Yıldız</t>
+          <t>Bahariye Cadde Eczanesi</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
           <t>
-+90 543 842 68 58</t>
++90 216 550 53 02</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
           <t>
-Mecidiye Mahallesi, Ortaköy, Muvakkit Sk. No:10/A, 34347 Beşiktaş/İstanbul, Türkiye</t>
+Osmanağa, Gen. Asım Gündüz Caddesi No:17/C, 34734 Kadıköy/İstanbul, Türkiye</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -550,19 +550,19 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Bahariye Cadde Eczanesi</t>
+          <t>İstanbul Eczanesi</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
           <t>
-+90 216 550 53 02</t>
++90 212 621 92 27</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
           <t>
-Osmanağa, Gen. Asım Gündüz Caddesi No:17/C, 34734 Kadıköy/İstanbul, Türkiye</t>
+Hırka-i Şerif, Kocasinan Cd. no: 90, 34091 Fatih/İstanbul, Türkiye</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -579,19 +579,19 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Colpan Pharmacy</t>
+          <t>Eczane Yıldız</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
           <t>
-+90 212 523 56 63</t>
++90 543 842 68 58</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
           <t>
-Akşemsettin, 34091 Fatih/İstanbul, Türkiye</t>
+Mecidiye Mahallesi, Ortaköy, Muvakkit Sk. No:10/A, 34347 Beşiktaş/İstanbul, Türkiye</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -608,19 +608,19 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>İstanbul Eczanesi</t>
+          <t>Colpan Pharmacy</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
           <t>
-+90 212 621 92 27</t>
++90 212 523 56 63</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
           <t>
-Hırka-i Şerif, Kocasinan Cd. no: 90, 34091 Fatih/İstanbul, Türkiye</t>
+Akşemsettin, 34091 Fatih/İstanbul, Türkiye</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -666,19 +666,19 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>İstanbul Havalimanı Eczane Melike Sultan</t>
+          <t>Istanbul Airport Pharmacy</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
           <t>
-+90 530 283 10 10</t>
++90 212 830 35 57</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
           <t>
-İstanbul AIRPORT Havalimanı Dış Hatlar Gelen Katı No:820540, İmrahor, 34283 Arnavutköy/İstanbul, Türkiye</t>
+Tayakadın Mah. İstanbul Yeni Havalimanı Giden Yolcu Katı NO: 7-F-0401, 34277 Arnavutköy/İstanbul, Türkiye</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
@@ -695,19 +695,19 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Istanbul Airport Pharmacy</t>
+          <t>İstanbul Havalimanı Eczane Melike Sultan</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
           <t>
-+90 212 830 35 57</t>
++90 530 283 10 10</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
           <t>
-Tayakadın Mah. İstanbul Yeni Havalimanı Giden Yolcu Katı NO: 7-F-0401, 34277 Arnavutköy/İstanbul, Türkiye</t>
+İstanbul AIRPORT Havalimanı Dış Hatlar Gelen Katı No:820540, İmrahor, 34283 Arnavutköy/İstanbul, Türkiye</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
@@ -724,17 +724,19 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Eczapaketim</t>
+          <t>Enes Eczanesi</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Yok</t>
+          <t>
++90 530 283 10 10</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Yok</t>
+          <t>
+İstanbul AIRPORT Havalimanı Dış Hatlar Gelen Katı No:820540, İmrahor, 34283 Arnavutköy/İstanbul, Türkiye</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Mon Feb  9 01:32:26 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E101"/>
+  <dimension ref="A1:E199"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3355,6 +3355,2847 @@
         </is>
       </c>
     </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Sahil Eczanesi</t>
+        </is>
+      </c>
+      <c r="B102" t="inlineStr">
+        <is>
+          <t>
++90 552 577 44 66</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>
+Fenerbahçe, Operatör Cemil Topuzlu Cd. Emek Apt No:39, 34000 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D102" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Bahariye Cadde Eczanesi</t>
+        </is>
+      </c>
+      <c r="B103" t="inlineStr">
+        <is>
+          <t>
++90 216 550 53 02</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Gen. Asım Gündüz Caddesi No:17/C, 34734 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D103" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Simirna Eczanesi</t>
+        </is>
+      </c>
+      <c r="B104" t="inlineStr">
+        <is>
+          <t>
++90 216 602 10 32</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Merdivenköy Cd No:29, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>ELİZYA ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B105" t="inlineStr">
+        <is>
+          <t>
++90 216 602 10 32</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Merdivenköy Cd No:29, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr">
+        <is>
+          <t>Bahariye Yavuz Eczanesi</t>
+        </is>
+      </c>
+      <c r="B106" t="inlineStr">
+        <is>
+          <t>
++90 216 602 10 32</t>
+        </is>
+      </c>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Merdivenköy Cd No:29, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr">
+        <is>
+          <t>Bilen Eczanesi</t>
+        </is>
+      </c>
+      <c r="B107" t="inlineStr">
+        <is>
+          <t>
++90 216 602 10 32</t>
+        </is>
+      </c>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Merdivenköy Cd No:29, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr">
+        <is>
+          <t>Caddebostan Nar Eczanesi - Ecz. Sibel Ozan</t>
+        </is>
+      </c>
+      <c r="B108" t="inlineStr">
+        <is>
+          <t>
++90 216 208 59 94</t>
+        </is>
+      </c>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>
+Kozyatağı, Kaya Sultan Sokağı 44/D, 34170 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr">
+        <is>
+          <t>Şifa Eczanesi</t>
+        </is>
+      </c>
+      <c r="B109" t="inlineStr">
+        <is>
+          <t>
++90 532 256 64 53</t>
+        </is>
+      </c>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>
+Dumlupınar, Mektep Sk. No: 16/D, 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr">
+        <is>
+          <t>Yeni Kadıköy Eczanesi</t>
+        </is>
+      </c>
+      <c r="B110" t="inlineStr">
+        <is>
+          <t>
++90 216 515 65 15</t>
+        </is>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Reşitefendi Sok. No:70/A, 34714 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr">
+        <is>
+          <t>Tuğba Karaca Eczanesi</t>
+        </is>
+      </c>
+      <c r="B111" t="inlineStr">
+        <is>
+          <t>
++90 216 566 11 91</t>
+        </is>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Şair Arşi Cd. No:11 A, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr">
+        <is>
+          <t>Sönmez Eczanesi</t>
+        </is>
+      </c>
+      <c r="B112" t="inlineStr">
+        <is>
+          <t>
++90 216 357 05 27</t>
+        </is>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Şemsettin Günaltay Cd. No:188 D:A, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr">
+        <is>
+          <t>HÜRRİYET ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B113" t="inlineStr">
+        <is>
+          <t>
++90 216 330 65 00</t>
+        </is>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Rıhtım Cd. 64/A, 34734 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr">
+        <is>
+          <t>Zeplin Eczanesi</t>
+        </is>
+      </c>
+      <c r="B114" t="inlineStr">
+        <is>
+          <t>
++90 533 925 34 00</t>
+        </is>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Serasker Cd. No:122/B, 34714 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr">
+        <is>
+          <t>Köşk Eczanesi</t>
+        </is>
+      </c>
+      <c r="B115" t="inlineStr">
+        <is>
+          <t>
++90 216 428 41 43</t>
+        </is>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>
+Hasanpaşa, Uzunçayır Cd. No:15, 34722 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr">
+        <is>
+          <t>Kadıköy Çarşı Eczanesi</t>
+        </is>
+      </c>
+      <c r="B116" t="inlineStr">
+        <is>
+          <t>
++90 216 338 48 38</t>
+        </is>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Tavus Sk. 18/b, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr">
+        <is>
+          <t>MERKEZ ECZANESİ (MERDİVENKÖY)</t>
+        </is>
+      </c>
+      <c r="B117" t="inlineStr">
+        <is>
+          <t>
++90 216 565 68 13</t>
+        </is>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Ressam Salih Erimez Cad No:7C, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="inlineStr">
+        <is>
+          <t>Moda Eczanesi</t>
+        </is>
+      </c>
+      <c r="B118" t="inlineStr">
+        <is>
+          <t>
++90 534 088 19 84</t>
+        </is>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Moda Cd. 83B, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="inlineStr">
+        <is>
+          <t>Akdeniz Eczanesi</t>
+        </is>
+      </c>
+      <c r="B119" t="inlineStr">
+        <is>
+          <t>
++90 534 088 19 84</t>
+        </is>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Moda Cd. 83B, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="inlineStr">
+        <is>
+          <t>Çarşı Zırhlıoğlu Eczanesi</t>
+        </is>
+      </c>
+      <c r="B120" t="inlineStr">
+        <is>
+          <t>
++90 534 088 19 84</t>
+        </is>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Moda Cd. 83B, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="inlineStr">
+        <is>
+          <t>Eczane Reva</t>
+        </is>
+      </c>
+      <c r="B121" t="inlineStr">
+        <is>
+          <t>
++90 534 088 19 84</t>
+        </is>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Moda Cd. 83B, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="inlineStr">
+        <is>
+          <t>SERASKER CADDE ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>
++90 534 088 19 84</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Moda Cd. 83B, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="inlineStr">
+        <is>
+          <t>eczane Serra</t>
+        </is>
+      </c>
+      <c r="B123" t="inlineStr">
+        <is>
+          <t>
++90 216 346 44 82</t>
+        </is>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Halitağa Cd. No:58, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="inlineStr">
+        <is>
+          <t>Eczane Altıyol Merkez</t>
+        </is>
+      </c>
+      <c r="B124" t="inlineStr">
+        <is>
+          <t>
++90 216 347 42 85</t>
+        </is>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Söğütlüçeşme Cad. NO:70-72, 34714 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="inlineStr">
+        <is>
+          <t>Kadıköy Eczanesi</t>
+        </is>
+      </c>
+      <c r="B125" t="inlineStr">
+        <is>
+          <t>
++90 543 899 92 44</t>
+        </is>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Kaptan Arif Sok. no:72A, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="inlineStr">
+        <is>
+          <t>Kent Eczanesi (Kent Plus Kadıköy)</t>
+        </is>
+      </c>
+      <c r="B126" t="inlineStr">
+        <is>
+          <t>
++90 216 969 42 48</t>
+        </is>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>
+KENT PLUS KADIKOY, Eğitim, Abdibey Sok. No:24/BH, 34722 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="inlineStr">
+        <is>
+          <t>Evranos Eczanesi</t>
+        </is>
+      </c>
+      <c r="B127" t="inlineStr">
+        <is>
+          <t>
++90 216 566 54 57</t>
+        </is>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>
+Göztepe, Nadirağa Sk. No:11/A, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="inlineStr">
+        <is>
+          <t>Kozmos Eczanesi</t>
+        </is>
+      </c>
+      <c r="B128" t="inlineStr">
+        <is>
+          <t>
++90 216 803 75 36</t>
+        </is>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Leylek Sok. 20 B, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="inlineStr">
+        <is>
+          <t>Mandarin Eczanesi</t>
+        </is>
+      </c>
+      <c r="B129" t="inlineStr">
+        <is>
+          <t>
++90 501 082 84 80</t>
+        </is>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>
+Fikirtepe Mah. Mandıra Cad. Mandarins No:11H, 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="inlineStr">
+        <is>
+          <t>Venüs Eczanesi</t>
+        </is>
+      </c>
+      <c r="B130" t="inlineStr">
+        <is>
+          <t>
++90 216 541 03 04</t>
+        </is>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>
+Fenerbahçe mh. Bağdat cd. Temel apt, no:146/A, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="inlineStr">
+        <is>
+          <t>Lokum Eczanesi / Pharmacy / Apotheke / аптека</t>
+        </is>
+      </c>
+      <c r="B131" t="inlineStr">
+        <is>
+          <t>
++90 216 348 12 13</t>
+        </is>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>
+Fenerbahçe, Lalezar Sk. No:5/A, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="inlineStr">
+        <is>
+          <t>MERKEZ NUR ECZANESI</t>
+        </is>
+      </c>
+      <c r="B132" t="inlineStr">
+        <is>
+          <t>
++90 216 346 81 51</t>
+        </is>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Söğütlüçeşme Cad. No:67, 34715 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="inlineStr">
+        <is>
+          <t>Zeytin Eczanesi</t>
+        </is>
+      </c>
+      <c r="B133" t="inlineStr">
+        <is>
+          <t>Yok</t>
+        </is>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Misak-ı Milli Sok. 81b, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="inlineStr">
+        <is>
+          <t>Birsu Eczanesi</t>
+        </is>
+      </c>
+      <c r="B134" t="inlineStr">
+        <is>
+          <t>
++90 216 565 64 41</t>
+        </is>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Moda Cd. 50/B, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="inlineStr">
+        <is>
+          <t>Sağlık Eczanesi</t>
+        </is>
+      </c>
+      <c r="B135" t="inlineStr">
+        <is>
+          <t>
++90 216 348 54 54</t>
+        </is>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Kuşdili Cd. No:45/A, 34714 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="inlineStr">
+        <is>
+          <t>GÖKTÜRK ECZANESİ (GÖKTÜRK PHARMACY)</t>
+        </is>
+      </c>
+      <c r="B136" t="inlineStr">
+        <is>
+          <t>
++90 216 325 50 17</t>
+        </is>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>
+Acıbadem, Sarayardı Cd. No: 1/A, 34660 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="inlineStr">
+        <is>
+          <t>19 Mayıs Eczanesi</t>
+        </is>
+      </c>
+      <c r="B137" t="inlineStr">
+        <is>
+          <t>
++90 216 380 77 66</t>
+        </is>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Hilmi Paşa Sk no:11B, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="inlineStr">
+        <is>
+          <t>Moda Zırhlıoğlu Eczanesi</t>
+        </is>
+      </c>
+      <c r="B138" t="inlineStr">
+        <is>
+          <t>
++90 216 449 19 75</t>
+        </is>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Moda Cd. No:193 D:1, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="inlineStr">
+        <is>
+          <t>Emre eczanesi</t>
+        </is>
+      </c>
+      <c r="B139" t="inlineStr">
+        <is>
+          <t>
++90 216 567 02 50</t>
+        </is>
+      </c>
+      <c r="C139" t="inlineStr">
+        <is>
+          <t>
+uğur apartmanı, Merdivenköy, Merdivenköy Cd no : 27/A, 34752 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="inlineStr">
+        <is>
+          <t>Halitağa Cadde Eczanesi</t>
+        </is>
+      </c>
+      <c r="B140" t="inlineStr">
+        <is>
+          <t>
++90 216 575 78 08</t>
+        </is>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Halitağa Cd. 36/A, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="inlineStr">
+        <is>
+          <t>Haydarpaşa Anadolu Eczanesi</t>
+        </is>
+      </c>
+      <c r="B141" t="inlineStr">
+        <is>
+          <t>
++90 216 339 60 45</t>
+        </is>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>
+Koşuyolu, Dr. Eyüp Aksoy Cd. No:37/B, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="inlineStr">
+        <is>
+          <t>VİTAMİN ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B142" t="inlineStr">
+        <is>
+          <t>
++90 216 349 33 34</t>
+        </is>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>
+Zühtüpaşa, Recep Peker Cd. NO:32 D:2a, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="inlineStr">
+        <is>
+          <t>Nar Ağacı Eczanesi</t>
+        </is>
+      </c>
+      <c r="B143" t="inlineStr">
+        <is>
+          <t>
++90 216 804 10 02</t>
+        </is>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>
+Feneryolu, Fahrettin Kerim Gökay Cd No:68 A, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="inlineStr">
+        <is>
+          <t>Feneryolu Eczanesi</t>
+        </is>
+      </c>
+      <c r="B144" t="inlineStr">
+        <is>
+          <t>
++90 216 345 52 26</t>
+        </is>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>
+Feneryolu, Gazi Muhtar Paşa Sk. No:34, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="inlineStr">
+        <is>
+          <t>Gülnur Eczanesi</t>
+        </is>
+      </c>
+      <c r="B145" t="inlineStr">
+        <is>
+          <t>
++90 216 411 48 45</t>
+        </is>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Bayar Cd. no : 41 D:1b, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="inlineStr">
+        <is>
+          <t>Ocak Eczanesi</t>
+        </is>
+      </c>
+      <c r="B146" t="inlineStr">
+        <is>
+          <t>
++90 216 449 96 27</t>
+        </is>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Rıhtım Cd. No:52, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="inlineStr">
+        <is>
+          <t>Akın Eczanesi</t>
+        </is>
+      </c>
+      <c r="B147" t="inlineStr">
+        <is>
+          <t>
++90 216 338 66 64</t>
+        </is>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Söğütlüçeşme Cad. No:121, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="inlineStr">
+        <is>
+          <t>Ayşe Lerzan Eczanesi</t>
+        </is>
+      </c>
+      <c r="B148" t="inlineStr">
+        <is>
+          <t>
++90 216 338 40 63</t>
+        </is>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Söğütlüçeşme Cad. No: 6/A, 34714 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="inlineStr">
+        <is>
+          <t>Yeni Nesil Eczanesi</t>
+        </is>
+      </c>
+      <c r="B149" t="inlineStr">
+        <is>
+          <t>
++90 216 357 03 04</t>
+        </is>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>
+Caddebostan, Tanzimat Sk. No:13/AKadıköy, 34728 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="inlineStr">
+        <is>
+          <t>Eczane Armanç</t>
+        </is>
+      </c>
+      <c r="B150" t="inlineStr">
+        <is>
+          <t>
++90 216 519 44 49</t>
+        </is>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>
+Fikirtepe, Rüzgar Sk. No:44/b-a, 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="inlineStr">
+        <is>
+          <t>Mungan Eczanesi</t>
+        </is>
+      </c>
+      <c r="B151" t="inlineStr">
+        <is>
+          <t>
++90 216 939 11 37</t>
+        </is>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>
+Kozyatağı, Kaya Sultan Sokağı No:21/b, 34742 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="inlineStr">
+        <is>
+          <t>AYBÜKE ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B152" t="inlineStr">
+        <is>
+          <t>
++90 216 339 78 82</t>
+        </is>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>
+Hasanpaşa, Arzu Sk. No:1, 34722, 34722 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="inlineStr">
+        <is>
+          <t>Mühürdar Eczanesi</t>
+        </is>
+      </c>
+      <c r="B153" t="inlineStr">
+        <is>
+          <t>
++90 216 405 22 91</t>
+        </is>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Mühürdar Cd. 48/A, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="inlineStr">
+        <is>
+          <t>ECZANE Sabuncu</t>
+        </is>
+      </c>
+      <c r="B154" t="inlineStr">
+        <is>
+          <t>
++90 216 345 91 15</t>
+        </is>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Nail Bey Sk. No:35, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="inlineStr">
+        <is>
+          <t>Flora Eczanesi</t>
+        </is>
+      </c>
+      <c r="B155" t="inlineStr">
+        <is>
+          <t>
++90 216 416 27 79</t>
+        </is>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Mercan Sk. No:5/A, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="inlineStr">
+        <is>
+          <t>Dünya Eczanesi</t>
+        </is>
+      </c>
+      <c r="B156" t="inlineStr">
+        <is>
+          <t>
++90 216 567 93 02</t>
+        </is>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>
+Feneryolu, Yıldıray Sk. No:2/B, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="inlineStr">
+        <is>
+          <t>KIZILTOPRAK ECZANESİ TESİS TARİHİ 1880</t>
+        </is>
+      </c>
+      <c r="B157" t="inlineStr">
+        <is>
+          <t>
++90 216 336 16 01</t>
+        </is>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>
+Fenerbahçe, Bağdat Cad. 54/A, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="inlineStr">
+        <is>
+          <t>Irmak Eczanesi</t>
+        </is>
+      </c>
+      <c r="B158" t="inlineStr">
+        <is>
+          <t>
++90 216 336 31 00</t>
+        </is>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>
+Zühtüpaşa, Recep Peker Cd. 34/A, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="inlineStr">
+        <is>
+          <t>NAUTILUS ECZANE</t>
+        </is>
+      </c>
+      <c r="B159" t="inlineStr">
+        <is>
+          <t>
++90 216 339 39 29</t>
+        </is>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>
+Tepe Nautilus, Acıbadem, Fatih Sk. No:1, 34718 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="inlineStr">
+        <is>
+          <t>Eczane Bahariye</t>
+        </is>
+      </c>
+      <c r="B160" t="inlineStr">
+        <is>
+          <t>
++90 216 336 74 05</t>
+        </is>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Sakız Gülü Sk. 31d, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="inlineStr">
+        <is>
+          <t>DOĞRUYOL ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>
++90 216 566 78 60</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>
+Feneryolu, Hüseyin Hüsnü Paşa Sk. No:3 D:B, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>Lotus 14 eczanesi</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>
++90 216 450 50 40</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Gen. Asım Gündüz Caddesi no:16A, 34714 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
+          <t>Aktürk Eczanesi Göztepe</t>
+        </is>
+      </c>
+      <c r="B163" t="inlineStr">
+        <is>
+          <t>
++90 216 478 13 13</t>
+        </is>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>
+Göztepe, Rıdvanpaşa Sok. No:5/A, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>Çiçek Eczanesi</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>
++90 216 369 00 19</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>
+Sahrayı Cedit, Kireçhaneler Sk. No:14/B, 34734 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>Elmas Eczanesi</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>
++90 216 405 19 00</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Karakolhane Cd. No:80, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>ECZANE YUNUS/PHARMACY YUNUS</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>
++90 216 565 94 88</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>
+ÖZEL Göztepe hastanesi, Merdivenköy caddesi, karşısı no:6/B, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>Eczane Güven</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>
++90 216 347 36 66</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Talimhane Sk. No:5, 34714 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>Seval Eczanesi</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>
++90 216 467 27 76</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>
+Sahrayı Cedit, İmam Ramiz Sokağı No:14, 34734 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Hızır Bey Eczanesi</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>
++90 507 661 71 85</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>
+HACI HASANBAŞ APT, Dumlupınar, Hızırbey Cd. no:207/B, 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="A170" t="inlineStr">
+        <is>
+          <t>Taniş Eczanesi</t>
+        </is>
+      </c>
+      <c r="B170" t="inlineStr">
+        <is>
+          <t>
++90 216 411 23 35</t>
+        </is>
+      </c>
+      <c r="C170" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Şemsettin Günaltay Cd. 20/A, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D170" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="A171" t="inlineStr">
+        <is>
+          <t>Melis Altınkaya Eczanesi</t>
+        </is>
+      </c>
+      <c r="B171" t="inlineStr">
+        <is>
+          <t>
++90 216 357 20 30</t>
+        </is>
+      </c>
+      <c r="C171" t="inlineStr">
+        <is>
+          <t>
+Fenerbahçe, Fuatpaşa Cd No:20, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D171" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="A172" t="inlineStr">
+        <is>
+          <t>Eczane Yurt</t>
+        </is>
+      </c>
+      <c r="B172" t="inlineStr">
+        <is>
+          <t>
++90 216 428 90 42</t>
+        </is>
+      </c>
+      <c r="C172" t="inlineStr">
+        <is>
+          <t>
+İbrahimağa Mah, Dr. Eyüp Aksoy Cd. 33/a, 34718 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D172" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="A173" t="inlineStr">
+        <is>
+          <t>Nurhan Eczanesi</t>
+        </is>
+      </c>
+      <c r="B173" t="inlineStr">
+        <is>
+          <t>
++90 216 346 69 89</t>
+        </is>
+      </c>
+      <c r="C173" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Güneşlibahçe Sok. 49/A, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D173" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="A174" t="inlineStr">
+        <is>
+          <t>ECZANE MELİS</t>
+        </is>
+      </c>
+      <c r="B174" t="inlineStr">
+        <is>
+          <t>
++90 216 355 06 70</t>
+        </is>
+      </c>
+      <c r="C174" t="inlineStr">
+        <is>
+          <t>
+Kadıköy Söğütlüçeşme caddesi, Yavuztürk Sk. 37B, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D174" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="A175" t="inlineStr">
+        <is>
+          <t>Lale Eczanesi (Fatih Lale)</t>
+        </is>
+      </c>
+      <c r="B175" t="inlineStr">
+        <is>
+          <t>
++90 216 565 98 22</t>
+        </is>
+      </c>
+      <c r="C175" t="inlineStr">
+        <is>
+          <t>
+Feneryolu, Fahrettin Kerim Gökay Cd NO:136/A, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D175" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="A176" t="inlineStr">
+        <is>
+          <t>Metin Çiçek Eczanesi</t>
+        </is>
+      </c>
+      <c r="B176" t="inlineStr">
+        <is>
+          <t>
++90 216 345 52 22</t>
+        </is>
+      </c>
+      <c r="C176" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Gen. Asım Gündüz Caddesi No:69/A, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D176" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="A177" t="inlineStr">
+        <is>
+          <t>ÇALIŞ ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B177" t="inlineStr">
+        <is>
+          <t>
++90 216 566 58 00</t>
+        </is>
+      </c>
+      <c r="C177" t="inlineStr">
+        <is>
+          <t>
+Dumlupınar, Hızırbey Cd. 207-A, 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D177" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="A178" t="inlineStr">
+        <is>
+          <t>Mavi Eczane</t>
+        </is>
+      </c>
+      <c r="B178" t="inlineStr">
+        <is>
+          <t>
++90 216 478 43 58</t>
+        </is>
+      </c>
+      <c r="C178" t="inlineStr">
+        <is>
+          <t>
+Caddebostan Opr.Dr. Cemil Topuzlu Caddesi No:109A (Plajyolu Sokak bitiminde, sağda. Cemil Topuzlu caddesi üzerinde, 34728 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D178" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="A179" t="inlineStr">
+        <is>
+          <t>Azim Eczanesi</t>
+        </is>
+      </c>
+      <c r="B179" t="inlineStr">
+        <is>
+          <t>
++90 216 336 61 63</t>
+        </is>
+      </c>
+      <c r="C179" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Süleyman Paşa Sk. No:6, 34714 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D179" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="A180" t="inlineStr">
+        <is>
+          <t>Kadıköy Merkez Eczanesi</t>
+        </is>
+      </c>
+      <c r="B180" t="inlineStr">
+        <is>
+          <t>
++90 534 648 20 80</t>
+        </is>
+      </c>
+      <c r="C180" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Muvakkıthane Cd. No:3, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D180" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="A181" t="inlineStr">
+        <is>
+          <t>Acıbadem Cadde Eczanesi</t>
+        </is>
+      </c>
+      <c r="B181" t="inlineStr">
+        <is>
+          <t>
++90 216 784 69 98</t>
+        </is>
+      </c>
+      <c r="C181" t="inlineStr">
+        <is>
+          <t>
+Acıbadem, Acıbadem Cd. no:47 A, 34718 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D181" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="A182" t="inlineStr">
+        <is>
+          <t>Kadir Eczanesi</t>
+        </is>
+      </c>
+      <c r="B182" t="inlineStr">
+        <is>
+          <t>
++90 216 629 55 80</t>
+        </is>
+      </c>
+      <c r="C182" t="inlineStr">
+        <is>
+          <t>
+Göztepe, Tütüncü Mehmet Efendi Cd. No:55C, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D182" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="A183" t="inlineStr">
+        <is>
+          <t>Sokak Eczanesi</t>
+        </is>
+      </c>
+      <c r="B183" t="inlineStr">
+        <is>
+          <t>
++90 216 337 67 37</t>
+        </is>
+      </c>
+      <c r="C183" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Karakolhane Cd. No:33/A, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D183" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="A184" t="inlineStr">
+        <is>
+          <t>Şebnem Eczanesi</t>
+        </is>
+      </c>
+      <c r="B184" t="inlineStr">
+        <is>
+          <t>
++90 216 325 88 98</t>
+        </is>
+      </c>
+      <c r="C184" t="inlineStr">
+        <is>
+          <t>
+Hasanpaşa, İkbaliye Sk., 34722 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D184" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="A185" t="inlineStr">
+        <is>
+          <t>Nihan Er Eczanesi Pharmacy</t>
+        </is>
+      </c>
+      <c r="B185" t="inlineStr">
+        <is>
+          <t>
++90 216 551 00 06</t>
+        </is>
+      </c>
+      <c r="C185" t="inlineStr">
+        <is>
+          <t>
+Fikirtepe, Mandıra Cd. No: 34/B, 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D185" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="A186" t="inlineStr">
+        <is>
+          <t>ECZANE TERMİNAL KADIKÖY</t>
+        </is>
+      </c>
+      <c r="B186" t="inlineStr">
+        <is>
+          <t>
++90 216 519 34 84</t>
+        </is>
+      </c>
+      <c r="C186" t="inlineStr">
+        <is>
+          <t>
+Hasanpaşa Mah. Kurbağalıdere Cad, Terminal Kadıköy'ün içerisinde, Marmaraya doğru giderken, Kahve Dünyası'nın yanında, Terminal No:2/8 İç Kapı No:3, 34722 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D186" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="A187" t="inlineStr">
+        <is>
+          <t>Şeniz Eczanesi</t>
+        </is>
+      </c>
+      <c r="B187" t="inlineStr">
+        <is>
+          <t>
++90 216 566 10 06</t>
+        </is>
+      </c>
+      <c r="C187" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Hızır Reis Sk., 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D187" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="A188" t="inlineStr">
+        <is>
+          <t>Derman Eczanesi</t>
+        </is>
+      </c>
+      <c r="B188" t="inlineStr">
+        <is>
+          <t>
++90 216 550 60 02</t>
+        </is>
+      </c>
+      <c r="C188" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Nemlizade Sk. 68/A, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D188" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="A189" t="inlineStr">
+        <is>
+          <t>Yeni İstanbul Eczanesi</t>
+        </is>
+      </c>
+      <c r="B189" t="inlineStr">
+        <is>
+          <t>
++90 216 416 61 71</t>
+        </is>
+      </c>
+      <c r="C189" t="inlineStr">
+        <is>
+          <t>
+Sahrayı Cedit, Bayar Cd. No:5 D:1A, 34734 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D189" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="A190" t="inlineStr">
+        <is>
+          <t>Sevda eczanesi</t>
+        </is>
+      </c>
+      <c r="B190" t="inlineStr">
+        <is>
+          <t>
++90 216 514 60 79</t>
+        </is>
+      </c>
+      <c r="C190" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Gürsoylu Sokağı no:32 D:34b, 34744 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D190" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="A191" t="inlineStr">
+        <is>
+          <t>Ezel Eczanesi</t>
+        </is>
+      </c>
+      <c r="B191" t="inlineStr">
+        <is>
+          <t>
++90 216 338 07 02</t>
+        </is>
+      </c>
+      <c r="C191" t="inlineStr">
+        <is>
+          <t>
+Zühtüpaşa, Itri Dede Sok. 23/A, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D191" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="A192" t="inlineStr">
+        <is>
+          <t>DURAK ECZANESİ KADIKÖY</t>
+        </is>
+      </c>
+      <c r="B192" t="inlineStr">
+        <is>
+          <t>
++90 534 662 81 97</t>
+        </is>
+      </c>
+      <c r="C192" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa Mah Rıhtım Cad N0:30 Sakıp Bey Apt Zemin Kat:1, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D192" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="A193" t="inlineStr">
+        <is>
+          <t>Sarayardı Eczanesi</t>
+        </is>
+      </c>
+      <c r="B193" t="inlineStr">
+        <is>
+          <t>
++90 216 428 54 80</t>
+        </is>
+      </c>
+      <c r="C193" t="inlineStr">
+        <is>
+          <t>
+Acıbadem, Sarayardı Cd. No:5 D:C, 34660 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D193" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="A194" t="inlineStr">
+        <is>
+          <t>VERDA ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B194" t="inlineStr">
+        <is>
+          <t>
++90 216 337 19 94</t>
+        </is>
+      </c>
+      <c r="C194" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Gen. Asım Gündüz Caddesi NO:104/A, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D194" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="A195" t="inlineStr">
+        <is>
+          <t>Lacivert Eczanesi</t>
+        </is>
+      </c>
+      <c r="B195" t="inlineStr">
+        <is>
+          <t>
++90 533 613 21 83</t>
+        </is>
+      </c>
+      <c r="C195" t="inlineStr">
+        <is>
+          <t>
+Feneryolu, Bağdat Cad. No:93, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D195" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="A196" t="inlineStr">
+        <is>
+          <t>Pınar Deniz Eczanesi</t>
+        </is>
+      </c>
+      <c r="B196" t="inlineStr">
+        <is>
+          <t>
++90 546 199 11 41</t>
+        </is>
+      </c>
+      <c r="C196" t="inlineStr">
+        <is>
+          <t>
+TEKNİK YAPI CONCORD İSTANBUL, Dumlupınar, Yumurtacı Abdi Bey Cd. C BLOK, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D196" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="A197" t="inlineStr">
+        <is>
+          <t>Toprak Eczanesi</t>
+        </is>
+      </c>
+      <c r="B197" t="inlineStr">
+        <is>
+          <t>
++90 541 899 97 99</t>
+        </is>
+      </c>
+      <c r="C197" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy Mahallesi Yumurtacı Abdi Bey Cad. B Blok No:5 Dikyol sok. No.2A (Business Istanbul) B Blok Daire No:5, 34732 Kadıköy, Türkiye</t>
+        </is>
+      </c>
+      <c r="D197" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="A198" t="inlineStr">
+        <is>
+          <t>Cumhuriyet Eczanesi</t>
+        </is>
+      </c>
+      <c r="B198" t="inlineStr">
+        <is>
+          <t>
++90 216 909 34 23</t>
+        </is>
+      </c>
+      <c r="C198" t="inlineStr">
+        <is>
+          <t>
+Göztepe, Tütüncü Mehmet Efendi Cd. No:13 D:A, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D198" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:32</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="A199" t="inlineStr">
+        <is>
+          <t>Naturel Eczanesi</t>
+        </is>
+      </c>
+      <c r="B199" t="inlineStr">
+        <is>
+          <t>
++90 216 909 34 23</t>
+        </is>
+      </c>
+      <c r="C199" t="inlineStr">
+        <is>
+          <t>
+Göztepe, Tütüncü Mehmet Efendi Cd. No:13 D:A, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D199" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>2026-02-09 01:32</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Tue Feb 10 01:51:05 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E199"/>
+  <dimension ref="A1:E212"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6196,6 +6196,383 @@
         </is>
       </c>
     </row>
+    <row r="200">
+      <c r="A200" t="inlineStr">
+        <is>
+          <t>Boğaziçi Eczanesi</t>
+        </is>
+      </c>
+      <c r="B200" t="inlineStr">
+        <is>
+          <t>
++90 538 357 12 52</t>
+        </is>
+      </c>
+      <c r="C200" t="inlineStr">
+        <is>
+          <t>
+Erenköy, General Necmi Ökten Sk. No: 14/A, 34738 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D200" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="A201" t="inlineStr">
+        <is>
+          <t>Sahrayıcedit Eczanesi</t>
+        </is>
+      </c>
+      <c r="B201" t="inlineStr">
+        <is>
+          <t>
++90 216 368 92 22</t>
+        </is>
+      </c>
+      <c r="C201" t="inlineStr">
+        <is>
+          <t>
+Sahrayı Cedit, Hafız İmam Sk. No:1 /1B, 34734 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D201" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="A202" t="inlineStr">
+        <is>
+          <t>Suadiye Eczanesi</t>
+        </is>
+      </c>
+      <c r="B202" t="inlineStr">
+        <is>
+          <t>
++90 216 380 40 40</t>
+        </is>
+      </c>
+      <c r="C202" t="inlineStr">
+        <is>
+          <t>
+Suadiye, Ayşeçavuş Cd No:7/C, 34740 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D202" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="A203" t="inlineStr">
+        <is>
+          <t>Eczane Halk</t>
+        </is>
+      </c>
+      <c r="B203" t="inlineStr">
+        <is>
+          <t>
++90 216 345 72 83</t>
+        </is>
+      </c>
+      <c r="C203" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Karakolhane Cd. No:11, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D203" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="A204" t="inlineStr">
+        <is>
+          <t>Aile Eczanesi</t>
+        </is>
+      </c>
+      <c r="B204" t="inlineStr">
+        <is>
+          <t>
++90 216 345 72 83</t>
+        </is>
+      </c>
+      <c r="C204" t="inlineStr">
+        <is>
+          <t>
+Rasimpaşa, Karakolhane Cd. No:11, 34716 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D204" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="A205" t="inlineStr">
+        <is>
+          <t>Utku Eczanesi</t>
+        </is>
+      </c>
+      <c r="B205" t="inlineStr">
+        <is>
+          <t>
++90 216 416 79 64</t>
+        </is>
+      </c>
+      <c r="C205" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Toktaş Sk. No:1 D:1 D, 34742 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D205" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="A206" t="inlineStr">
+        <is>
+          <t>Kaptan Eczanesi</t>
+        </is>
+      </c>
+      <c r="B206" t="inlineStr">
+        <is>
+          <t>
++90 216 416 79 64</t>
+        </is>
+      </c>
+      <c r="C206" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Toktaş Sk. No:1 D:1 D, 34742 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D206" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="A207" t="inlineStr">
+        <is>
+          <t>Tılsım Eczanesi</t>
+        </is>
+      </c>
+      <c r="B207" t="inlineStr">
+        <is>
+          <t>
++90 216 416 79 64</t>
+        </is>
+      </c>
+      <c r="C207" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Toktaş Sk. No:1 D:1 D, 34742 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D207" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="A208" t="inlineStr">
+        <is>
+          <t>İdeal Eczanesi Kadıköy</t>
+        </is>
+      </c>
+      <c r="B208" t="inlineStr">
+        <is>
+          <t>
++90 216 416 79 64</t>
+        </is>
+      </c>
+      <c r="C208" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Toktaş Sk. No:1 D:1 D, 34742 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D208" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="A209" t="inlineStr">
+        <is>
+          <t>Cansever Eczanesi</t>
+        </is>
+      </c>
+      <c r="B209" t="inlineStr">
+        <is>
+          <t>
++90 216 347 00 92</t>
+        </is>
+      </c>
+      <c r="C209" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Moda Cd. No:21/B, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D209" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="A210" t="inlineStr">
+        <is>
+          <t>Dalyan Eczanesi</t>
+        </is>
+      </c>
+      <c r="B210" t="inlineStr">
+        <is>
+          <t>
++90 216 359 86 06</t>
+        </is>
+      </c>
+      <c r="C210" t="inlineStr">
+        <is>
+          <t>
+Fenerbahçe, Operatör Cemil Topuzlu Cd. No:4 F Blok, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D210" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="A211" t="inlineStr">
+        <is>
+          <t>Buket Eczanesi</t>
+        </is>
+      </c>
+      <c r="B211" t="inlineStr">
+        <is>
+          <t>
++90 216 360 32 92</t>
+        </is>
+      </c>
+      <c r="C211" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Tekkealtı Sk. Nuribey Apt. 4/B, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D211" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:51</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="A212" t="inlineStr">
+        <is>
+          <t>PERA ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B212" t="inlineStr">
+        <is>
+          <t>
++90 216 766 11 53</t>
+        </is>
+      </c>
+      <c r="C212" t="inlineStr">
+        <is>
+          <t>
+Erenköy, Ethemefendi Caddesi No:26, 34738 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D212" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>2026-02-10 01:51</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Wed Feb 11 01:47:56 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E212"/>
+  <dimension ref="A1:E222"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6573,6 +6573,296 @@
         </is>
       </c>
     </row>
+    <row r="213">
+      <c r="A213" t="inlineStr">
+        <is>
+          <t>Soley Eczanesi</t>
+        </is>
+      </c>
+      <c r="B213" t="inlineStr">
+        <is>
+          <t>
++90 506 598 90 50</t>
+        </is>
+      </c>
+      <c r="C213" t="inlineStr">
+        <is>
+          <t>
+Bostancı, Kozyatağı, Seda Sk. No:11/A, 34742 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D213" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>2026-02-11 01:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="A214" t="inlineStr">
+        <is>
+          <t>CADDE SAĞLIK ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B214" t="inlineStr">
+        <is>
+          <t>
++90 216 356 00 85</t>
+        </is>
+      </c>
+      <c r="C214" t="inlineStr">
+        <is>
+          <t>
+CADDE SAĞLIK ECZANESİ, Caddebostan, Bağdat Cad. NO:275 D:1, 34728 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D214" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>2026-02-11 01:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="A215" t="inlineStr">
+        <is>
+          <t>Alp Eczanesi</t>
+        </is>
+      </c>
+      <c r="B215" t="inlineStr">
+        <is>
+          <t>
++90 546 128 82 46</t>
+        </is>
+      </c>
+      <c r="C215" t="inlineStr">
+        <is>
+          <t>
+Erenköy, Kamiller Sokağı No:5 D:B, 34738 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D215" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>2026-02-11 01:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="A216" t="inlineStr">
+        <is>
+          <t>Karaca Eczanesi</t>
+        </is>
+      </c>
+      <c r="B216" t="inlineStr">
+        <is>
+          <t>
++90 216 748 08 88</t>
+        </is>
+      </c>
+      <c r="C216" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Oral Sk. No: 1/B, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D216" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>2026-02-11 01:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="A217" t="inlineStr">
+        <is>
+          <t>GÖKÇEN ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B217" t="inlineStr">
+        <is>
+          <t>
++90 216 629 86 06</t>
+        </is>
+      </c>
+      <c r="C217" t="inlineStr">
+        <is>
+          <t>
+Dumlupınar, Yazıcılar Sk., 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D217" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>2026-02-11 01:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="A218" t="inlineStr">
+        <is>
+          <t>Eczane Ertem</t>
+        </is>
+      </c>
+      <c r="B218" t="inlineStr">
+        <is>
+          <t>
++90 216 338 84 98</t>
+        </is>
+      </c>
+      <c r="C218" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Moda Cd. No:112, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D218" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>2026-02-11 01:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="219">
+      <c r="A219" t="inlineStr">
+        <is>
+          <t>Eczane Nihal</t>
+        </is>
+      </c>
+      <c r="B219" t="inlineStr">
+        <is>
+          <t>
++90 216 368 42 14</t>
+        </is>
+      </c>
+      <c r="C219" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Sinan Ercan Cd. No:30 C, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D219" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E219" t="inlineStr">
+        <is>
+          <t>2026-02-11 01:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="220">
+      <c r="A220" t="inlineStr">
+        <is>
+          <t>Eczane Saye</t>
+        </is>
+      </c>
+      <c r="B220" t="inlineStr">
+        <is>
+          <t>
++90 216 360 85 93</t>
+        </is>
+      </c>
+      <c r="C220" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Yıldız Sk. No:15/B, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D220" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E220" t="inlineStr">
+        <is>
+          <t>2026-02-11 01:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="221">
+      <c r="A221" t="inlineStr">
+        <is>
+          <t>Güleç Eczanesi</t>
+        </is>
+      </c>
+      <c r="B221" t="inlineStr">
+        <is>
+          <t>
++90 216 909 26 96</t>
+        </is>
+      </c>
+      <c r="C221" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Yıldız Sk. No:18/B, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D221" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E221" t="inlineStr">
+        <is>
+          <t>2026-02-11 01:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="222">
+      <c r="A222" t="inlineStr">
+        <is>
+          <t>Ergenekon Eczanesi</t>
+        </is>
+      </c>
+      <c r="B222" t="inlineStr">
+        <is>
+          <t>
++90 216 414 65 83</t>
+        </is>
+      </c>
+      <c r="C222" t="inlineStr">
+        <is>
+          <t>
+Zühtüpaşa, Kördere Sok. 22/A, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D222" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E222" t="inlineStr">
+        <is>
+          <t>2026-02-11 01:47</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Thu Feb 12 01:27:52 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E222"/>
+  <dimension ref="A1:E227"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6863,6 +6863,151 @@
         </is>
       </c>
     </row>
+    <row r="223">
+      <c r="A223" t="inlineStr">
+        <is>
+          <t>ECZANE Vatan</t>
+        </is>
+      </c>
+      <c r="B223" t="inlineStr">
+        <is>
+          <t>
++90 216 565 96 71</t>
+        </is>
+      </c>
+      <c r="C223" t="inlineStr">
+        <is>
+          <t>
+Dumlupınar Mh.şahika sok.no:1/C FİKİRTEPE, 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D223" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>2026-02-12 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="224">
+      <c r="A224" t="inlineStr">
+        <is>
+          <t>Pelikan Eczanesi</t>
+        </is>
+      </c>
+      <c r="B224" t="inlineStr">
+        <is>
+          <t>
++90 530 765 82 94</t>
+        </is>
+      </c>
+      <c r="C224" t="inlineStr">
+        <is>
+          <t>
+Göztepe, Tütüncü Mehmet Efendi Cd. 107/B, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D224" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>2026-02-12 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="225">
+      <c r="A225" t="inlineStr">
+        <is>
+          <t>Ecem Ramiz Eczanesi</t>
+        </is>
+      </c>
+      <c r="B225" t="inlineStr">
+        <is>
+          <t>
++90 216 337 09 19</t>
+        </is>
+      </c>
+      <c r="C225" t="inlineStr">
+        <is>
+          <t>
+Göztepe, Nadirağa Sk. No:5-7E D:F, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D225" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E225" t="inlineStr">
+        <is>
+          <t>2026-02-12 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="226">
+      <c r="A226" t="inlineStr">
+        <is>
+          <t>Caddebostan Plus Eczanesi</t>
+        </is>
+      </c>
+      <c r="B226" t="inlineStr">
+        <is>
+          <t>
++90 545 350 10 00</t>
+        </is>
+      </c>
+      <c r="C226" t="inlineStr">
+        <is>
+          <t>
+Caddebostan, Ömer Paşa Sk. no:1, 34728 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D226" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E226" t="inlineStr">
+        <is>
+          <t>2026-02-12 01:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="227">
+      <c r="A227" t="inlineStr">
+        <is>
+          <t>Kekik Eczanesi</t>
+        </is>
+      </c>
+      <c r="B227" t="inlineStr">
+        <is>
+          <t>
++90 216 356 78 91</t>
+        </is>
+      </c>
+      <c r="C227" t="inlineStr">
+        <is>
+          <t>
+Atatürk Caddesi Makbule Apt. No.37/A Sahrayıcedit, 34734 İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D227" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E227" t="inlineStr">
+        <is>
+          <t>2026-02-12 01:27</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Sat Feb 14 01:22:01 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E227"/>
+  <dimension ref="A1:E228"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7008,6 +7008,35 @@
         </is>
       </c>
     </row>
+    <row r="228">
+      <c r="A228" t="inlineStr">
+        <is>
+          <t>Elit Eczanesi</t>
+        </is>
+      </c>
+      <c r="B228" t="inlineStr">
+        <is>
+          <t>
++90 216 363 20 20</t>
+        </is>
+      </c>
+      <c r="C228" t="inlineStr">
+        <is>
+          <t>
+Göztepe, Bağdat Cad. No:209/A, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D228" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E228" t="inlineStr">
+        <is>
+          <t>2026-02-14 01:22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Sun Feb 15 01:30:25 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E228"/>
+  <dimension ref="A1:E230"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7037,6 +7037,63 @@
         </is>
       </c>
     </row>
+    <row r="229">
+      <c r="A229" t="inlineStr">
+        <is>
+          <t>Aybüke İrem Eczanesi</t>
+        </is>
+      </c>
+      <c r="B229" t="inlineStr">
+        <is>
+          <t>
++90 216 567 17 57</t>
+        </is>
+      </c>
+      <c r="C229" t="inlineStr">
+        <is>
+          <t>
+Feneryolu Mah, Göztepe, Fahrettin Kerim Gökay Cd NO:138A, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D229" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E229" t="inlineStr">
+        <is>
+          <t>2026-02-15 01:29</t>
+        </is>
+      </c>
+    </row>
+    <row r="230">
+      <c r="A230" t="inlineStr">
+        <is>
+          <t>Nihan Eczanesi</t>
+        </is>
+      </c>
+      <c r="B230" t="inlineStr">
+        <is>
+          <t>Yok</t>
+        </is>
+      </c>
+      <c r="C230" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Dr. Erkin Cd. No:10, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D230" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E230" t="inlineStr">
+        <is>
+          <t>2026-02-15 01:30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Mon Feb 16 01:26:30 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E230"/>
+  <dimension ref="A1:E250"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7094,6 +7094,586 @@
         </is>
       </c>
     </row>
+    <row r="231">
+      <c r="A231" t="inlineStr">
+        <is>
+          <t>Eczane Ecrin</t>
+        </is>
+      </c>
+      <c r="B231" t="inlineStr">
+        <is>
+          <t>
++90 216 566 20 21</t>
+        </is>
+      </c>
+      <c r="C231" t="inlineStr">
+        <is>
+          <t>
+ÖZEL GÖZTEPE MEDİCALPARK HASTANESİ YANI, Merdivenköy, Nisan Sk. NO:20/A, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D231" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E231" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="232">
+      <c r="A232" t="inlineStr">
+        <is>
+          <t>Bostancı Eczanesi</t>
+        </is>
+      </c>
+      <c r="B232" t="inlineStr">
+        <is>
+          <t>
++90 850 677 5616</t>
+        </is>
+      </c>
+      <c r="C232" t="inlineStr">
+        <is>
+          <t>
+Bostancı, Prof. Dr. Ali Nihat Tarlan Cd No:54/B, 34744 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D232" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E232" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="233">
+      <c r="A233" t="inlineStr">
+        <is>
+          <t>Eczane Coşan</t>
+        </is>
+      </c>
+      <c r="B233" t="inlineStr">
+        <is>
+          <t>
++90 216 357 19 19</t>
+        </is>
+      </c>
+      <c r="C233" t="inlineStr">
+        <is>
+          <t>
+Fenerbahçe, Tevfik Paşa Sk. No:2 D:1C, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D233" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E233" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="234">
+      <c r="A234" t="inlineStr">
+        <is>
+          <t>Eczane Ülkü</t>
+        </is>
+      </c>
+      <c r="B234" t="inlineStr">
+        <is>
+          <t>
++90 216 356 49 64</t>
+        </is>
+      </c>
+      <c r="C234" t="inlineStr">
+        <is>
+          <t>
+Sahrayı Cedit, İnönü Cd. 6/B, 34734 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D234" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E234" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="235">
+      <c r="A235" t="inlineStr">
+        <is>
+          <t>Fenerbahçe Beyaz Eczane</t>
+        </is>
+      </c>
+      <c r="B235" t="inlineStr">
+        <is>
+          <t>
++90 216 345 08 11</t>
+        </is>
+      </c>
+      <c r="C235" t="inlineStr">
+        <is>
+          <t>
+Fenerbahçe, Fener Kalamış Cd. No:92-94 / D, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D235" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E235" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="236">
+      <c r="A236" t="inlineStr">
+        <is>
+          <t>Nazan Eczane</t>
+        </is>
+      </c>
+      <c r="B236" t="inlineStr">
+        <is>
+          <t>
++90 216 411 84 82</t>
+        </is>
+      </c>
+      <c r="C236" t="inlineStr">
+        <is>
+          <t>
+19 Mayıs, Şemsettin Günaltay Cd. No:174, 34736 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D236" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E236" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="237">
+      <c r="A237" t="inlineStr">
+        <is>
+          <t>Eczane İskele</t>
+        </is>
+      </c>
+      <c r="B237" t="inlineStr">
+        <is>
+          <t>
++90 216 336 61 10</t>
+        </is>
+      </c>
+      <c r="C237" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Rıhtım Cd. No:2, 34714 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D237" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E237" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="238">
+      <c r="A238" t="inlineStr">
+        <is>
+          <t>Eczane Mısra Kan</t>
+        </is>
+      </c>
+      <c r="B238" t="inlineStr">
+        <is>
+          <t>
++90 216 385 00 96</t>
+        </is>
+      </c>
+      <c r="C238" t="inlineStr">
+        <is>
+          <t>
+Erenköy, Şemsettin Günaltay Cd. no:173/c, 34738 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D238" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E238" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="239">
+      <c r="A239" t="inlineStr">
+        <is>
+          <t>İntepe Eczanesi</t>
+        </is>
+      </c>
+      <c r="B239" t="inlineStr">
+        <is>
+          <t>
++90 216 445 07 26</t>
+        </is>
+      </c>
+      <c r="C239" t="inlineStr">
+        <is>
+          <t>
+Kozyatağı, Korkut Sk. 6B, 34742 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D239" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E239" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="240">
+      <c r="A240" t="inlineStr">
+        <is>
+          <t>Ece Bayram Eczanesi</t>
+        </is>
+      </c>
+      <c r="B240" t="inlineStr">
+        <is>
+          <t>
++90 216 629 48 80</t>
+        </is>
+      </c>
+      <c r="C240" t="inlineStr">
+        <is>
+          <t>
+Feneryolu, Bağdat Cad. No:71A, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D240" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E240" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="241">
+      <c r="A241" t="inlineStr">
+        <is>
+          <t>HEKİMOĞLU ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B241" t="inlineStr">
+        <is>
+          <t>
++90 216 385 85 87</t>
+        </is>
+      </c>
+      <c r="C241" t="inlineStr">
+        <is>
+          <t>
+Erenköy, Telli Kavak Sk. No:1, 34334 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D241" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E241" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="242">
+      <c r="A242" t="inlineStr">
+        <is>
+          <t>ŞEYMA CANER ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B242" t="inlineStr">
+        <is>
+          <t>
++90 216 784 11 93</t>
+        </is>
+      </c>
+      <c r="C242" t="inlineStr">
+        <is>
+          <t>
+Fenerbahçe, Fener Kalamış Cd. No:67 D:1B, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D242" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E242" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="243">
+      <c r="A243" t="inlineStr">
+        <is>
+          <t>Pırlanta eczane</t>
+        </is>
+      </c>
+      <c r="B243" t="inlineStr">
+        <is>
+          <t>
++90 216 771 00 00</t>
+        </is>
+      </c>
+      <c r="C243" t="inlineStr">
+        <is>
+          <t>
+Dumlupınar Mahallesi, Hızırbey Cd, Dumlupınar, Adagül Sk. No:4, 34720, Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D243" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E243" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="244">
+      <c r="A244" t="inlineStr">
+        <is>
+          <t>Yalçın Eczanesi Feneryolu</t>
+        </is>
+      </c>
+      <c r="B244" t="inlineStr">
+        <is>
+          <t>
++90 216 338 67 29</t>
+        </is>
+      </c>
+      <c r="C244" t="inlineStr">
+        <is>
+          <t>
+Feneryolu, Fenerbahçe, Bağdat Cad. No:119/B, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D244" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E244" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="245">
+      <c r="A245" t="inlineStr">
+        <is>
+          <t>Burkay Eczanesi</t>
+        </is>
+      </c>
+      <c r="B245" t="inlineStr">
+        <is>
+          <t>
++90 216 567 22 22</t>
+        </is>
+      </c>
+      <c r="C245" t="inlineStr">
+        <is>
+          <t>
+Mustafa Kaya Sokağı, Göztepe, Fahrettin Kerim Gökay Cd no:18/b, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D245" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="246">
+      <c r="A246" t="inlineStr">
+        <is>
+          <t>Emine Eczanesi</t>
+        </is>
+      </c>
+      <c r="B246" t="inlineStr">
+        <is>
+          <t>
++90 216 386 04 89</t>
+        </is>
+      </c>
+      <c r="C246" t="inlineStr">
+        <is>
+          <t>
+Erenköy, Çoban Yıldızı Sokağı no12/b, 34738 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D246" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="247">
+      <c r="A247" t="inlineStr">
+        <is>
+          <t>Nova Eczanesi</t>
+        </is>
+      </c>
+      <c r="B247" t="inlineStr">
+        <is>
+          <t>
++90 216 766 01 94</t>
+        </is>
+      </c>
+      <c r="C247" t="inlineStr">
+        <is>
+          <t>
+Suadiye, Halay Sk. No:12/B, 34740 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D247" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E247" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="248">
+      <c r="A248" t="inlineStr">
+        <is>
+          <t>Vega Eczanesi Kadıköy</t>
+        </is>
+      </c>
+      <c r="B248" t="inlineStr">
+        <is>
+          <t>
++90 532 668 83 42</t>
+        </is>
+      </c>
+      <c r="C248" t="inlineStr">
+        <is>
+          <t>
+Göztepe, Ömer Paşa Sk. UZAY APT NO27/A, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D248" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E248" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="249">
+      <c r="A249" t="inlineStr">
+        <is>
+          <t>LAGÜN ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B249" t="inlineStr">
+        <is>
+          <t>
++90 216 999 00 93</t>
+        </is>
+      </c>
+      <c r="C249" t="inlineStr">
+        <is>
+          <t>
+Göztepe, Tepegöz Sk. NO:5/A, 34730 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D249" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E249" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="250">
+      <c r="A250" t="inlineStr">
+        <is>
+          <t>ONİKİLER ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B250" t="inlineStr">
+        <is>
+          <t>
++90 216 567 62 58</t>
+        </is>
+      </c>
+      <c r="C250" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Dr. Erkin Cd. 58/A, 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D250" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E250" t="inlineStr">
+        <is>
+          <t>2026-02-16 01:26</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Tue Feb 17 01:25:12 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E250"/>
+  <dimension ref="A1:E252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7674,6 +7674,64 @@
         </is>
       </c>
     </row>
+    <row r="251">
+      <c r="A251" t="inlineStr">
+        <is>
+          <t>MEYDAN ECZANESİ-PHARMACY</t>
+        </is>
+      </c>
+      <c r="B251" t="inlineStr">
+        <is>
+          <t>
++90 501 240 22 33</t>
+        </is>
+      </c>
+      <c r="C251" t="inlineStr">
+        <is>
+          <t>
+Osmanağa, Söğütlüçeşme Cad. No:57, 34714 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D251" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E251" t="inlineStr">
+        <is>
+          <t>2026-02-17 01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="252">
+      <c r="A252" t="inlineStr">
+        <is>
+          <t>Aktaş Eczanesi</t>
+        </is>
+      </c>
+      <c r="B252" t="inlineStr">
+        <is>
+          <t>
++90 216 567 24 42</t>
+        </is>
+      </c>
+      <c r="C252" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Dr. Erkin Cd. Sefa Apt. 16/18-a, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D252" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E252" t="inlineStr">
+        <is>
+          <t>2026-02-17 01:25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Wed Feb 18 01:27:52 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E252"/>
+  <dimension ref="A1:E253"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7732,6 +7732,35 @@
         </is>
       </c>
     </row>
+    <row r="253">
+      <c r="A253" t="inlineStr">
+        <is>
+          <t>ACIBADEM ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B253" t="inlineStr">
+        <is>
+          <t>
++90 216 545 58 45</t>
+        </is>
+      </c>
+      <c r="C253" t="inlineStr">
+        <is>
+          <t>
+Acıbadem, Mustafa Bey Sk. No:1/A, 34718 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D253" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>2026-02-18 01:27</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Thu Feb 19 01:26:52 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E253"/>
+  <dimension ref="A1:E254"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7761,6 +7761,35 @@
         </is>
       </c>
     </row>
+    <row r="254">
+      <c r="A254" t="inlineStr">
+        <is>
+          <t>Gümüş Eczanesi</t>
+        </is>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>
++90 216 330 41 82</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>
+Feneryolu, Gazi Muhtar Paşa Sk. No:59 D:I, 34726 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D254" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>2026-02-19 01:26</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Fri Feb 20 01:22:56 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E254"/>
+  <dimension ref="A1:E255"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7790,6 +7790,35 @@
         </is>
       </c>
     </row>
+    <row r="255">
+      <c r="A255" t="inlineStr">
+        <is>
+          <t>Aslı Eczanesi</t>
+        </is>
+      </c>
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>
++90 216 550 04 91</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>
+Eğitim, Nahitbey Sok. 51/A, 34722 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D255" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E255" t="inlineStr">
+        <is>
+          <t>2026-02-20 01:22</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Sat Feb 21 01:20:48 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E255"/>
+  <dimension ref="A1:E257"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7819,6 +7819,64 @@
         </is>
       </c>
     </row>
+    <row r="256">
+      <c r="A256" t="inlineStr">
+        <is>
+          <t>Alfa Eczanesi</t>
+        </is>
+      </c>
+      <c r="B256" t="inlineStr">
+        <is>
+          <t>
++90 216 339 43 39</t>
+        </is>
+      </c>
+      <c r="C256" t="inlineStr">
+        <is>
+          <t>
+Koşuyolu, Koşuyolu Cd. No:2/A, 34718 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D256" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E256" t="inlineStr">
+        <is>
+          <t>2026-02-21 01:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="257">
+      <c r="A257" t="inlineStr">
+        <is>
+          <t>ECZANE TEKDEMİR</t>
+        </is>
+      </c>
+      <c r="B257" t="inlineStr">
+        <is>
+          <t>
++90 216 565 35 61</t>
+        </is>
+      </c>
+      <c r="C257" t="inlineStr">
+        <is>
+          <t>
+Merdivenköy, Şahika Sk. 33/A, 34732 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D257" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E257" t="inlineStr">
+        <is>
+          <t>2026-02-21 01:20</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Sun Feb 22 01:25:59 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E257"/>
+  <dimension ref="A1:E258"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7877,6 +7877,35 @@
         </is>
       </c>
     </row>
+    <row r="258">
+      <c r="A258" t="inlineStr">
+        <is>
+          <t>MODA SAHİL ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B258" t="inlineStr">
+        <is>
+          <t>
++90 533 022 94 91</t>
+        </is>
+      </c>
+      <c r="C258" t="inlineStr">
+        <is>
+          <t>
+Caferağa, Ferit Tek Sok. NO60/C, 34710 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D258" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E258" t="inlineStr">
+        <is>
+          <t>2026-02-22 01:25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Mon Feb 23 01:25:24 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E258"/>
+  <dimension ref="A1:E260"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7906,6 +7906,64 @@
         </is>
       </c>
     </row>
+    <row r="259">
+      <c r="A259" t="inlineStr">
+        <is>
+          <t>Asil Eczanesi</t>
+        </is>
+      </c>
+      <c r="B259" t="inlineStr">
+        <is>
+          <t>
++90 546 960 61 77</t>
+        </is>
+      </c>
+      <c r="C259" t="inlineStr">
+        <is>
+          <t>
+Feneryolu, Feneryolu Sokağı No:20/C-D, 34724 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D259" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E259" t="inlineStr">
+        <is>
+          <t>2026-02-23 01:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="260">
+      <c r="A260" t="inlineStr">
+        <is>
+          <t>ENES UYGUN ECZANESİ</t>
+        </is>
+      </c>
+      <c r="B260" t="inlineStr">
+        <is>
+          <t>
++90 216 361 09 27</t>
+        </is>
+      </c>
+      <c r="C260" t="inlineStr">
+        <is>
+          <t>
+Kozyatağı, Kaya Sultan Sokağı 28/A, 34742 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D260" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E260" t="inlineStr">
+        <is>
+          <t>2026-02-23 01:25</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Tue Feb 24 01:24:17 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E260"/>
+  <dimension ref="A1:E261"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7964,6 +7964,35 @@
         </is>
       </c>
     </row>
+    <row r="261">
+      <c r="A261" t="inlineStr">
+        <is>
+          <t>Cadde 360 Eczanesi</t>
+        </is>
+      </c>
+      <c r="B261" t="inlineStr">
+        <is>
+          <t>
++90 216 358 09 68</t>
+        </is>
+      </c>
+      <c r="C261" t="inlineStr">
+        <is>
+          <t>
+Caddebostan, Bağdat Cad. 327/A, 34728 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D261" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E261" t="inlineStr">
+        <is>
+          <t>2026-02-24 01:24</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Wed Feb 25 01:30:13 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E261"/>
+  <dimension ref="A1:E262"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7993,6 +7993,35 @@
         </is>
       </c>
     </row>
+    <row r="262">
+      <c r="A262" t="inlineStr">
+        <is>
+          <t>Kare Eczanesi</t>
+        </is>
+      </c>
+      <c r="B262" t="inlineStr">
+        <is>
+          <t>
++90 533 372 40 39</t>
+        </is>
+      </c>
+      <c r="C262" t="inlineStr">
+        <is>
+          <t>
+Fikirtepe, Barış Sokak No:7AF, 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D262" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E262" t="inlineStr">
+        <is>
+          <t>2026-02-25 01:30</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Thu Feb 26 01:23:40 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E262"/>
+  <dimension ref="A1:E263"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8022,6 +8022,35 @@
         </is>
       </c>
     </row>
+    <row r="263">
+      <c r="A263" t="inlineStr">
+        <is>
+          <t>Kozyatağı Eczanesi</t>
+        </is>
+      </c>
+      <c r="B263" t="inlineStr">
+        <is>
+          <t>
++90 216 747 30 33</t>
+        </is>
+      </c>
+      <c r="C263" t="inlineStr">
+        <is>
+          <t>
+şemsettin günaltay no:114/B Ayşekadın, Kozyatağı, Şemsettin Günaltay Cd. no:114/B, 34742 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D263" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E263" t="inlineStr">
+        <is>
+          <t>2026-02-26 01:23</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Sat Feb 28 01:15:50 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E263"/>
+  <dimension ref="A1:E265"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8051,6 +8051,64 @@
         </is>
       </c>
     </row>
+    <row r="264">
+      <c r="A264" t="inlineStr">
+        <is>
+          <t>Ömerpaşa Eczanesi</t>
+        </is>
+      </c>
+      <c r="B264" t="inlineStr">
+        <is>
+          <t>
++90 533 724 06 74</t>
+        </is>
+      </c>
+      <c r="C264" t="inlineStr">
+        <is>
+          <t>
+Sahrayı Cedit, Ferit Bey Sk. no:6/c, 34744 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D264" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E264" t="inlineStr">
+        <is>
+          <t>2026-02-28 01:15</t>
+        </is>
+      </c>
+    </row>
+    <row r="265">
+      <c r="A265" t="inlineStr">
+        <is>
+          <t>Aqua Eczanesi</t>
+        </is>
+      </c>
+      <c r="B265" t="inlineStr">
+        <is>
+          <t>
++90 216 771 19 98</t>
+        </is>
+      </c>
+      <c r="C265" t="inlineStr">
+        <is>
+          <t>
+Caddebostan, Operatör Cemil Topuzlu Cd. No:139/A, 34728 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D265" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E265" t="inlineStr">
+        <is>
+          <t>2026-02-28 01:15</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Sun Mar  1 01:43:37 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E265"/>
+  <dimension ref="A1:E267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8109,6 +8109,64 @@
         </is>
       </c>
     </row>
+    <row r="266">
+      <c r="A266" t="inlineStr">
+        <is>
+          <t>Altanlar Eczanesi</t>
+        </is>
+      </c>
+      <c r="B266" t="inlineStr">
+        <is>
+          <t>
++90 216 410 44 06</t>
+        </is>
+      </c>
+      <c r="C266" t="inlineStr">
+        <is>
+          <t>
+Suadiye, Ayşeçavuş Cd 21/A, 34740 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D266" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E266" t="inlineStr">
+        <is>
+          <t>2026-03-01 01:43</t>
+        </is>
+      </c>
+    </row>
+    <row r="267">
+      <c r="A267" t="inlineStr">
+        <is>
+          <t>Selin Eczanesi</t>
+        </is>
+      </c>
+      <c r="B267" t="inlineStr">
+        <is>
+          <t>
++90 542 108 47 24</t>
+        </is>
+      </c>
+      <c r="C267" t="inlineStr">
+        <is>
+          <t>
+Dumlupınar, Adagül Sk. Köseoğlu Apt No:2/B, 34720 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D267" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E267" t="inlineStr">
+        <is>
+          <t>2026-03-01 01:43</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
✅ Veri Güncellendi:  - Mon Mar  2 01:23:33 UTC 2026
</commit_message>
<xml_diff>
--- a/leads_output.xlsx
+++ b/leads_output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E267"/>
+  <dimension ref="A1:E269"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8167,6 +8167,64 @@
         </is>
       </c>
     </row>
+    <row r="268">
+      <c r="A268" t="inlineStr">
+        <is>
+          <t>Atlas Eczanesi</t>
+        </is>
+      </c>
+      <c r="B268" t="inlineStr">
+        <is>
+          <t>
++90 216 771 10 12</t>
+        </is>
+      </c>
+      <c r="C268" t="inlineStr">
+        <is>
+          <t>
+Sahrayı Cedit, İnönü Cd. No:14/A, 34734 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D268" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E268" t="inlineStr">
+        <is>
+          <t>2026-03-02 01:23</t>
+        </is>
+      </c>
+    </row>
+    <row r="269">
+      <c r="A269" t="inlineStr">
+        <is>
+          <t>Gülerman Eczanesi</t>
+        </is>
+      </c>
+      <c r="B269" t="inlineStr">
+        <is>
+          <t>
++90 216 467 12 38</t>
+        </is>
+      </c>
+      <c r="C269" t="inlineStr">
+        <is>
+          <t>
+Erenköy, Erenköy İstasyon Cd. No:11 C, 34738 Kadıköy/İstanbul, Türkiye</t>
+        </is>
+      </c>
+      <c r="D269" t="inlineStr">
+        <is>
+          <t>Kadikoy/Istanbul</t>
+        </is>
+      </c>
+      <c r="E269" t="inlineStr">
+        <is>
+          <t>2026-03-02 01:23</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>